<commit_message>
created and then detached excitation component. currently not working
</commit_message>
<xml_diff>
--- a/car_rig_data.xlsx
+++ b/car_rig_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\GitHub\DS-C_B-Half-Car-Rig-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD5E38A-3056-4C76-9EDA-CEC6DC2A38E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CC3047-55DA-45F5-8DAA-FFC3BAD21249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,18 +53,6 @@
     <t>I1 (kgm^2)</t>
   </si>
   <si>
-    <t>K1 (kN/m)</t>
-  </si>
-  <si>
-    <t>K2 (kN/m)</t>
-  </si>
-  <si>
-    <t>K3 (kN/m)</t>
-  </si>
-  <si>
-    <t>K4 (kN/m)</t>
-  </si>
-  <si>
     <t>C1 (Ns/m)</t>
   </si>
   <si>
@@ -81,6 +69,18 @@
   </si>
   <si>
     <t>L2 (m)</t>
+  </si>
+  <si>
+    <t>K1 (N/m)</t>
+  </si>
+  <si>
+    <t>K2 (N/m)</t>
+  </si>
+  <si>
+    <t>K3 (N/m)</t>
+  </si>
+  <si>
+    <t>K4 (N/m)</t>
   </si>
 </sst>
 </file>
@@ -401,7 +401,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,71 +444,75 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>20.5</v>
+        <f>20.5*1000</f>
+        <v>20500</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>20.5</v>
+        <f>20.5*1000</f>
+        <v>20500</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>147.19999999999999</v>
+        <f>147.2*1000</f>
+        <v>147200</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8">
-        <v>147.19999999999999</v>
+        <f>147.2*1000</f>
+        <v>147200</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13">
         <v>0.75</v>
@@ -516,7 +520,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>0.75</v>
@@ -527,7 +531,8 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <v>12.5</v>
+        <f>12.5*1000</f>
+        <v>12500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added initial variable support
</commit_message>
<xml_diff>
--- a/car_rig_data.xlsx
+++ b/car_rig_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\GitHub\DS-C_B-Half-Car-Rig-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CC3047-55DA-45F5-8DAA-FFC3BAD21249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACA1E39-1A20-4783-B7F8-538B9A789004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5130" yWindow="5880" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +531,6 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <f>12.5*1000</f>
         <v>12500</v>
       </c>
     </row>

</xml_diff>